<commit_message>
new map, text edits for Stephanie
</commit_message>
<xml_diff>
--- a/word/Table2.xlsx
+++ b/word/Table2.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\docs\manuscripts\cali_analysis\word\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\manuscripts\cali_analysis\word\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18405" windowHeight="10260"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18405" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,17 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Models</t>
   </si>
   <si>
-    <t>Bacteria</t>
-  </si>
-  <si>
-    <t>Archaea</t>
-  </si>
-  <si>
     <t>Constant (close)</t>
   </si>
   <si>
@@ -59,58 +53,38 @@
     <t>Adjusted R2</t>
   </si>
   <si>
-    <t>85.97∗∗∗</t>
-  </si>
-  <si>
-    <t>3.42∗∗∗</t>
-  </si>
-  <si>
-    <t>−0.06</t>
-  </si>
-  <si>
     <t>−22.05∗∗∗</t>
   </si>
   <si>
-    <t>−14.25∗∗</t>
-  </si>
-  <si>
-    <t>−0.08</t>
-  </si>
-  <si>
-    <t>8.74∗∗∗</t>
-  </si>
-  <si>
-    <t>∗p&lt;0.1; ∗∗p&lt;0.05; ∗∗∗p&lt;0.01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Note: </t>
-  </si>
-  <si>
-    <t>Table 2: Summary of analysis of variance results for bacteria and archaea diversity with distance from outflow. Diversity measures were based on Fisher’s Alpha (Fisher et al. 1943) using abundance of genera at each site. The model intercept is the average diversity estimate (standard error in parentheses) at all close sites and the remaining parameter estimates (intermediate and farthest) are referenced accordingly.</t>
-  </si>
-  <si>
-    <t>(-3.78)</t>
-  </si>
-  <si>
-    <t>(-4.9)</t>
-  </si>
-  <si>
-    <t>(-5.37)</t>
-  </si>
-  <si>
-    <t>(-0.59)</t>
-  </si>
-  <si>
-    <t>(-0.76)</t>
-  </si>
-  <si>
-    <t>(-0.84)</t>
+    <t xml:space="preserve">Note: ∗p&lt;0.1; ∗∗p&lt;0.05; ∗∗∗p&lt;0.01
+</t>
+  </si>
+  <si>
+    <t>Table 2: Summary of analysis of variance results for community diversity with distance from outflow. Diversity measures were based on Fisher’s Alpha (Fisher et al. 1943) using abundance of genera at each site. The model intercept is the average diversity estimate (standard error in parentheses) at all close sites and the remaining parameter estimates (intermediate and farthest) are referenced accordingly.</t>
+  </si>
+  <si>
+    <t>88.68∗∗∗</t>
+  </si>
+  <si>
+    <t>−14.72∗∗</t>
+  </si>
+  <si>
+    <t>8.63∗∗∗</t>
+  </si>
+  <si>
+    <t>(5.01)</t>
+  </si>
+  <si>
+    <t>(3.88)</t>
+  </si>
+  <si>
+    <t>(5.48)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -140,20 +114,11 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -181,33 +146,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,173 +494,124 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="19.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="35.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4" t="s">
+    <row r="1" spans="1:2" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="B3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="B5" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="B7" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="B9" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B12" s="6">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="8">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="8">
-        <v>14</v>
-      </c>
-      <c r="C10" s="8">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="8">
-        <v>0.61</v>
-      </c>
-      <c r="C11" s="8">
-        <v>0.09</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+    </row>
+    <row r="14" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="8">
-        <v>0.54</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="8">
-        <v>7.59</v>
-      </c>
-      <c r="C13" s="8">
-        <v>1.18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="6">
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="9"/>
-      <c r="D15"/>
+      <c r="B14"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="A1:C1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>